<commit_message>
Mapping sheets, USDM version update for v4
</commit_message>
<xml_diff>
--- a/Documents/Mappings/ct-gov_mapping.xlsx
+++ b/Documents/Mappings/ct-gov_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_mapping/final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/GitHub/DDF-RA/Documents/Mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C996E61-39F7-5E46-8666-97AB73C683C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5651516B-7589-A94B-9C7E-3FCF56B03053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68700" yWindow="4640" windowWidth="29400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
     <t>In some cases there is more than one mapping for the same M11 item. These mappings are usually distinct where either one of them may be used (and the other is expected to be not available) or they need to be all combined for the M11 item.</t>
   </si>
   <si>
-    <t>v3.13</t>
+    <t>v4.0.0</t>
   </si>
 </sst>
 </file>
@@ -1319,6 +1319,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1342,51 +1387,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1696,7 +1696,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1863,29 +1865,29 @@
     <col min="9" max="9" width="71" customWidth="1"/>
     <col min="10" max="10" width="36.5" customWidth="1"/>
     <col min="11" max="12" width="25.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" style="47" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="47" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="39" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1924,10 +1926,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1964,10 +1966,10 @@
       <c r="L3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="46" t="s">
+      <c r="M3" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2004,10 +2006,10 @@
       <c r="L4" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="M4" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="46"/>
+      <c r="M4" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="38"/>
     </row>
     <row r="5" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
@@ -2042,10 +2044,10 @@
       <c r="L5" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="M5" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="46"/>
+      <c r="M5" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="38"/>
     </row>
     <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
@@ -2080,10 +2082,10 @@
       <c r="L6" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="M6" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="46"/>
+      <c r="M6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
@@ -2116,10 +2118,10 @@
       <c r="L7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="46" t="s">
+      <c r="M7" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2156,10 +2158,10 @@
       <c r="L8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="46" t="s">
+      <c r="M8" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2194,10 +2196,10 @@
       <c r="L9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="46" t="s">
+      <c r="M9" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2230,10 +2232,10 @@
       <c r="L10" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="M10" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="46" t="s">
+      <c r="M10" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2275,29 +2277,29 @@
     <col min="9" max="9" width="45.83203125" customWidth="1"/>
     <col min="10" max="10" width="42.33203125" customWidth="1"/>
     <col min="11" max="12" width="25.5" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="47" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" style="47" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="39" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" ht="22" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -2336,10 +2338,10 @@
       <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="40" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2366,10 +2368,10 @@
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="49" t="s">
+      <c r="M3" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="41" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2402,10 +2404,10 @@
       <c r="L4" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M4" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="49" t="s">
+      <c r="M4" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2440,10 +2442,10 @@
       <c r="L5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M5" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="49" t="s">
+      <c r="M5" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2478,10 +2480,10 @@
       <c r="L6" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M6" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="49" t="s">
+      <c r="M6" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2516,10 +2518,10 @@
       <c r="L7" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M7" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="49" t="s">
+      <c r="M7" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2552,10 +2554,10 @@
       <c r="L8" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="49" t="s">
+      <c r="M8" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2590,10 +2592,10 @@
       <c r="L9" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="49" t="s">
+      <c r="M9" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2610,8 +2612,8 @@
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2647,28 +2649,28 @@
     <col min="6" max="6" width="25.83203125" style="29" customWidth="1"/>
     <col min="7" max="10" width="43.6640625" style="29" customWidth="1"/>
     <col min="11" max="12" width="25.83203125" style="29" customWidth="1"/>
-    <col min="13" max="14" width="17.1640625" style="55" customWidth="1"/>
+    <col min="13" max="14" width="17.1640625" style="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2707,10 +2709,10 @@
       <c r="L2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2744,10 +2746,10 @@
       <c r="L3" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M3" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="49" t="s">
+      <c r="M3" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2781,10 +2783,10 @@
       <c r="L4" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M4" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="49" t="s">
+      <c r="M4" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2821,10 +2823,10 @@
       <c r="L5" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="49" t="s">
+      <c r="M5" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2858,10 +2860,10 @@
       <c r="L6" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="M6" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="49" t="s">
+      <c r="M6" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2900,10 +2902,10 @@
       <c r="L7" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M7" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="52"/>
+      <c r="M7" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="44"/>
     </row>
     <row r="8" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -2940,10 +2942,10 @@
       <c r="L8" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="M8" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="49" t="s">
+      <c r="M8" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2980,10 +2982,10 @@
       <c r="L9" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="M9" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="49" t="s">
+      <c r="M9" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="41" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3022,10 +3024,10 @@
       <c r="L10" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M10" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="52"/>
+      <c r="M10" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="44"/>
     </row>
     <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -3062,10 +3064,10 @@
       <c r="L11" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M11" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="52"/>
+      <c r="M11" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="44"/>
     </row>
     <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -3102,10 +3104,10 @@
       <c r="L12" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="M12" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" s="52"/>
+      <c r="M12" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="44"/>
     </row>
     <row r="13" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -3142,10 +3144,10 @@
       <c r="L13" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="M13" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" s="52"/>
+      <c r="M13" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="44"/>
     </row>
     <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -3182,10 +3184,10 @@
       <c r="L14" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M14" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="49" t="s">
+      <c r="M14" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3224,10 +3226,10 @@
       <c r="L15" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M15" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="49" t="s">
+      <c r="M15" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3266,10 +3268,10 @@
       <c r="L16" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="M16" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" s="49" t="s">
+      <c r="M16" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3308,10 +3310,10 @@
       <c r="L17" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="M17" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="49" t="s">
+      <c r="M17" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3350,10 +3352,10 @@
       <c r="L18" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="M18" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" s="49" t="s">
+      <c r="M18" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3392,10 +3394,10 @@
       <c r="L19" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="M19" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="N19" s="49" t="s">
+      <c r="M19" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3420,8 +3422,8 @@
       <c r="J20" s="4"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="49" t="s">
+      <c r="M20" s="44"/>
+      <c r="N20" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3460,10 +3462,10 @@
       <c r="L21" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="M21" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21" s="49" t="s">
+      <c r="M21" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21" s="41" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3500,30 +3502,30 @@
     <col min="8" max="8" width="39" style="7" customWidth="1"/>
     <col min="9" max="10" width="43.1640625" style="7" customWidth="1"/>
     <col min="11" max="12" width="32.6640625" style="7" customWidth="1"/>
-    <col min="13" max="14" width="16.83203125" style="56" customWidth="1"/>
+    <col min="13" max="14" width="16.83203125" style="48" customWidth="1"/>
     <col min="15" max="16" width="21.5" style="7" customWidth="1"/>
     <col min="17" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3562,10 +3564,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3604,10 +3606,10 @@
       <c r="L3" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M3" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="49"/>
+      <c r="M3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="41"/>
     </row>
     <row r="4" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -3644,10 +3646,10 @@
       <c r="L4" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="49"/>
+      <c r="M4" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="41"/>
     </row>
     <row r="5" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -3684,10 +3686,10 @@
       <c r="L5" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="49"/>
+      <c r="M5" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="41"/>
     </row>
     <row r="6" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -3726,10 +3728,10 @@
       <c r="L6" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="M6" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="49"/>
+      <c r="M6" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="41"/>
     </row>
     <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -3766,10 +3768,10 @@
       <c r="L7" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="M7" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="49"/>
+      <c r="M7" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="41"/>
     </row>
     <row r="8" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -3806,10 +3808,10 @@
       <c r="L8" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="M8" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="49" t="s">
+      <c r="M8" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="41" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3850,10 +3852,10 @@
       <c r="L9" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="M9" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="49" t="s">
+      <c r="M9" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="41" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3878,10 +3880,10 @@
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="49" t="s">
+      <c r="M10" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="N10" s="49" t="s">
+      <c r="N10" s="41" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3918,10 +3920,10 @@
       <c r="L11" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="M11" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="49" t="s">
+      <c r="M11" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="41" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3946,10 +3948,10 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="49" t="s">
+      <c r="M12" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="N12" s="49" t="s">
+      <c r="N12" s="41" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3981,30 +3983,30 @@
     <col min="9" max="9" width="38.1640625" style="35" customWidth="1"/>
     <col min="10" max="10" width="21.5" style="35" customWidth="1"/>
     <col min="11" max="12" width="32.6640625" style="35" customWidth="1"/>
-    <col min="13" max="14" width="16.1640625" style="58" customWidth="1"/>
+    <col min="13" max="14" width="16.1640625" style="50" customWidth="1"/>
     <col min="15" max="16" width="21.5" style="7" customWidth="1"/>
     <col min="17" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4043,10 +4045,10 @@
       <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4087,10 +4089,10 @@
       <c r="L3" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="M3" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="57" t="s">
+      <c r="M3" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4115,10 +4117,10 @@
       <c r="J4" s="3"/>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N4" s="57" t="s">
+      <c r="N4" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4143,10 +4145,10 @@
       <c r="I5" s="3"/>
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4187,10 +4189,10 @@
       <c r="L6" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="M6" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="57" t="s">
+      <c r="M6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4215,10 +4217,10 @@
       <c r="J7" s="3"/>
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
-      <c r="M7" s="57" t="s">
+      <c r="M7" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N7" s="57" t="s">
+      <c r="N7" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4243,10 +4245,10 @@
       <c r="I8" s="3"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
-      <c r="M8" s="57" t="s">
+      <c r="M8" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N8" s="57" t="s">
+      <c r="N8" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4287,10 +4289,10 @@
       <c r="L9" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="M9" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="57"/>
+      <c r="M9" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="49"/>
     </row>
     <row r="10" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -4313,10 +4315,10 @@
       <c r="J10" s="3"/>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N10" s="57" t="s">
+      <c r="N10" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4342,10 +4344,10 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
-      <c r="M11" s="57" t="s">
+      <c r="M11" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="N11" s="57" t="s">
+      <c r="N11" s="49" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4377,30 +4379,30 @@
     <col min="9" max="9" width="35" style="8" customWidth="1"/>
     <col min="10" max="10" width="39" style="8" customWidth="1"/>
     <col min="11" max="12" width="24.33203125" style="8" customWidth="1"/>
-    <col min="13" max="14" width="19" style="59" customWidth="1"/>
+    <col min="13" max="14" width="19" style="51" customWidth="1"/>
     <col min="15" max="16" width="21.5" style="8" customWidth="1"/>
     <col min="17" max="16384" width="8.6640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14" ht="22" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
@@ -4439,10 +4441,10 @@
       <c r="L2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="40" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4483,10 +4485,10 @@
       <c r="L3" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M3" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="46"/>
+      <c r="M3" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="38"/>
     </row>
     <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
@@ -4523,10 +4525,10 @@
       <c r="L4" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M4" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="46" t="s">
+      <c r="M4" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="38" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4559,10 +4561,10 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="41" t="s">
         <v>296</v>
       </c>
-      <c r="N5" s="51" t="s">
+      <c r="N5" s="43" t="s">
         <v>254</v>
       </c>
     </row>
@@ -4601,10 +4603,10 @@
       <c r="L6" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M6" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="46"/>
+      <c r="M6" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="38"/>
     </row>
     <row r="7" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -4641,10 +4643,10 @@
       <c r="L7" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M7" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="46"/>
+      <c r="M7" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="38"/>
     </row>
     <row r="8" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -4683,10 +4685,10 @@
       <c r="L8" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M8" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="46"/>
+      <c r="M8" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -4725,10 +4727,10 @@
       <c r="L9" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M9" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="46"/>
+      <c r="M9" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="38"/>
     </row>
     <row r="10" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
@@ -4765,10 +4767,10 @@
       <c r="L10" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M10" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="46"/>
+      <c r="M10" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="38"/>
     </row>
     <row r="11" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
@@ -4805,10 +4807,10 @@
       <c r="L11" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M11" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="46"/>
+      <c r="M11" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="38"/>
     </row>
     <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
@@ -4847,10 +4849,10 @@
       <c r="L12" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M12" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N12" s="46"/>
+      <c r="M12" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="38"/>
     </row>
     <row r="13" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
@@ -4889,10 +4891,10 @@
       <c r="L13" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M13" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" s="46"/>
+      <c r="M13" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="38"/>
     </row>
     <row r="14" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
@@ -4929,10 +4931,10 @@
       <c r="L14" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M14" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="46"/>
+      <c r="M14" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="38"/>
     </row>
     <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
@@ -4969,10 +4971,10 @@
       <c r="L15" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M15" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="46"/>
+      <c r="M15" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="38"/>
     </row>
     <row r="16" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
@@ -5009,10 +5011,10 @@
       <c r="L16" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="M16" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" s="46"/>
+      <c r="M16" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="38"/>
     </row>
     <row r="17" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
@@ -5051,10 +5053,10 @@
       <c r="L17" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="M17" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="46"/>
+      <c r="M17" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="38"/>
     </row>
     <row r="18" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
@@ -5091,10 +5093,10 @@
       <c r="L18" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="M18" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="N18" s="46" t="s">
+      <c r="M18" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="38" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>